<commit_message>
create missing commodity case for AVA-C (ACTFLO)
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_NewTechs.xlsx
+++ b/SubRES_TMPL/SubRES_NewTechs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\DemoS_ADV_Stuttgart061118\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF16DC8-CFC3-4B43-ACBF-E28EC9FB45D7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB60CD-5284-43BE-9644-A5E7343879D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5955" yWindow="570" windowWidth="22185" windowHeight="15030" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELC" sheetId="4" r:id="rId1"/>
@@ -26,15 +26,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -2022,7 +2014,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="259">
   <si>
     <t>~FI_T</t>
   </si>
@@ -2345,9 +2337,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>ACTFLO~DEMO</t>
-  </si>
-  <si>
     <t>Activity to Flo</t>
   </si>
   <si>
@@ -2796,6 +2785,12 @@
   </si>
   <si>
     <t>AF</t>
+  </si>
+  <si>
+    <t>CommGrp</t>
+  </si>
+  <si>
+    <t>ACTFLO</t>
   </si>
 </sst>
 </file>
@@ -4968,7 +4963,7 @@
         <v>53</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>55</v>
@@ -5162,7 +5157,7 @@
         <v>70</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N11" s="17" t="s">
         <v>72</v>
@@ -5224,7 +5219,7 @@
         <v>41</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M12" s="19" t="s">
         <v>38</v>
@@ -5343,10 +5338,10 @@
       </c>
       <c r="Q14" s="114"/>
       <c r="R14" s="114" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="S14" s="114" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="T14" s="114" t="s">
         <v>52</v>
@@ -5401,10 +5396,10 @@
       <c r="P15" s="114"/>
       <c r="Q15" s="114"/>
       <c r="R15" s="114" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="S15" s="114" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="T15" s="114" t="s">
         <v>52</v>
@@ -5460,10 +5455,10 @@
       <c r="P16" s="114"/>
       <c r="Q16" s="114"/>
       <c r="R16" s="114" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="S16" s="114" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="T16" s="114" t="s">
         <v>52</v>
@@ -5491,10 +5486,10 @@
       <c r="P17" s="114"/>
       <c r="Q17" s="114"/>
       <c r="R17" s="114" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="S17" s="117" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T17" s="114" t="s">
         <v>52</v>
@@ -5520,10 +5515,10 @@
       <c r="P18" s="114"/>
       <c r="Q18" s="114"/>
       <c r="R18" s="114" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="S18" s="117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="T18" s="114" t="s">
         <v>52</v>
@@ -5549,10 +5544,10 @@
       <c r="P19" s="114"/>
       <c r="Q19" s="114"/>
       <c r="R19" s="114" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S19" s="117" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="T19" s="114" t="s">
         <v>52</v>
@@ -5566,10 +5561,10 @@
     </row>
     <row r="20" spans="2:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>249</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>250</v>
       </c>
       <c r="D20" s="27" t="s">
         <v>49</v>
@@ -5605,10 +5600,10 @@
       <c r="P20" s="114"/>
       <c r="Q20" s="114"/>
       <c r="R20" s="114" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S20" s="117" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="T20" s="114" t="s">
         <v>52</v>
@@ -5626,7 +5621,7 @@
         <v>ELCRNBIO01</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>49</v>
@@ -5659,14 +5654,14 @@
         <v>1</v>
       </c>
       <c r="P21" s="118" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q21" s="114"/>
       <c r="R21" s="119" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S21" s="117" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="T21" s="114" t="s">
         <v>52</v>
@@ -5675,7 +5670,7 @@
         <v>53</v>
       </c>
       <c r="V21" s="115" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W21" s="114"/>
       <c r="X21" s="114"/>
@@ -5686,7 +5681,7 @@
         <v>ELCRNHYD01</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D22" s="25" t="s">
         <v>49</v>
@@ -5732,7 +5727,7 @@
         <v>ELCRNWIN01</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>49</v>
@@ -5780,7 +5775,7 @@
         <v>ELCRNSOL01</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>49</v>
@@ -5930,7 +5925,7 @@
     </row>
     <row r="4" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="51" t="s">
         <v>100</v>
@@ -5943,10 +5938,10 @@
         <v>52</v>
       </c>
       <c r="F4" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="51" t="s">
         <v>124</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>125</v>
       </c>
       <c r="I4" s="51" t="s">
         <v>55</v>
@@ -6182,7 +6177,7 @@
         <v>41</v>
       </c>
       <c r="L12" s="61" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M12" s="61" t="s">
         <v>38</v>
@@ -6470,7 +6465,7 @@
         <v>52</v>
       </c>
       <c r="G2" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K2" s="108" t="s">
         <v>7</v>
@@ -6588,13 +6583,13 @@
         <v>11</v>
       </c>
       <c r="G8" s="76" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="76" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="76" t="s">
+      <c r="I8" s="76" t="s">
         <v>127</v>
-      </c>
-      <c r="I8" s="76" t="s">
-        <v>128</v>
       </c>
       <c r="J8" s="8"/>
       <c r="K8" s="110" t="s">
@@ -6639,13 +6634,13 @@
       <c r="E9" s="72"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72" t="s">
+        <v>128</v>
+      </c>
+      <c r="H9" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="72" t="s">
+      <c r="I9" s="72" t="s">
         <v>130</v>
-      </c>
-      <c r="I9" s="72" t="s">
-        <v>131</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="112" t="s">
@@ -6689,7 +6684,7 @@
         <v>52</v>
       </c>
       <c r="H10" s="74" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I10" s="74" t="s">
         <v>52</v>
@@ -7086,7 +7081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -7145,10 +7140,10 @@
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D4" s="44" t="s">
         <v>94</v>
@@ -7157,10 +7152,10 @@
         <v>52</v>
       </c>
       <c r="F4" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="40" t="s">
         <v>124</v>
-      </c>
-      <c r="H4" s="40" t="s">
-        <v>125</v>
       </c>
       <c r="I4" s="40" t="s">
         <v>55</v>
@@ -7168,10 +7163,10 @@
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>135</v>
       </c>
       <c r="D5" s="44" t="s">
         <v>94</v>
@@ -7183,7 +7178,7 @@
         <v>53</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I5" s="51" t="s">
         <v>55</v>
@@ -7218,7 +7213,7 @@
         <v>53</v>
       </c>
       <c r="H6" s="51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I6" s="51" t="s">
         <v>55</v>
@@ -7359,7 +7354,7 @@
         <v>35</v>
       </c>
       <c r="H12" s="82" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I12" s="18" t="s">
         <v>39</v>
@@ -7425,7 +7420,7 @@
         <v>40</v>
       </c>
       <c r="K13" s="45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M13" s="112" t="s">
         <v>77</v>
@@ -7465,13 +7460,13 @@
       <c r="F14" s="47"/>
       <c r="G14" s="48"/>
       <c r="H14" s="85" t="s">
+        <v>153</v>
+      </c>
+      <c r="I14" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="I14" s="47" t="s">
+      <c r="J14" s="47" t="s">
         <v>155</v>
-      </c>
-      <c r="J14" s="47" t="s">
-        <v>156</v>
       </c>
       <c r="K14" s="47" t="s">
         <v>84</v>
@@ -7494,10 +7489,10 @@
         <v>CSHNCOA1</v>
       </c>
       <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" t="s">
         <v>136</v>
-      </c>
-      <c r="D15" t="s">
-        <v>137</v>
       </c>
       <c r="E15" s="36">
         <v>2006</v>
@@ -7525,10 +7520,10 @@
       </c>
       <c r="N15" s="114"/>
       <c r="O15" s="114" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P15" s="121" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="Q15" s="114" t="s">
         <v>52</v>
@@ -7546,10 +7541,10 @@
         <v>CSHNGAS1</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E16" s="36">
         <v>2006</v>
@@ -7575,10 +7570,10 @@
       <c r="M16" s="114"/>
       <c r="N16" s="114"/>
       <c r="O16" s="114" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="P16" s="121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q16" s="114" t="s">
         <v>52</v>
@@ -7596,10 +7591,10 @@
         <v>CSHNOIL1</v>
       </c>
       <c r="C17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E17" s="36">
         <v>2006</v>
@@ -7625,10 +7620,10 @@
       <c r="M17" s="114"/>
       <c r="N17" s="114"/>
       <c r="O17" s="114" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="P17" s="121" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="Q17" s="114" t="s">
         <v>52</v>
@@ -7646,10 +7641,10 @@
         <v>CSHNBIO1</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="36">
         <v>2006</v>
@@ -7675,10 +7670,10 @@
       <c r="M18" s="114"/>
       <c r="N18" s="114"/>
       <c r="O18" s="114" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="P18" s="121" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="Q18" s="114" t="s">
         <v>52</v>
@@ -7696,10 +7691,10 @@
         <v>CSHNSOL1</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E19" s="36">
         <v>2006</v>
@@ -7725,10 +7720,10 @@
       <c r="M19" s="114"/>
       <c r="N19" s="114"/>
       <c r="O19" s="114" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P19" s="121" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Q19" s="114" t="s">
         <v>52</v>
@@ -7746,10 +7741,10 @@
         <v>CSHNELC1</v>
       </c>
       <c r="C20" s="86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D20" s="86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E20" s="36">
         <v>2006</v>
@@ -7775,10 +7770,10 @@
       <c r="M20" s="114"/>
       <c r="N20" s="114"/>
       <c r="O20" s="114" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P20" s="121" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q20" s="114" t="s">
         <v>52</v>
@@ -7796,10 +7791,10 @@
         <v>CAPNELC1</v>
       </c>
       <c r="C21" s="87" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="87" t="s">
         <v>140</v>
-      </c>
-      <c r="D21" s="87" t="s">
-        <v>141</v>
       </c>
       <c r="E21" s="93">
         <v>2006</v>
@@ -7823,10 +7818,10 @@
       <c r="M21" s="114"/>
       <c r="N21" s="114"/>
       <c r="O21" s="114" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P21" s="121" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q21" s="114" t="s">
         <v>52</v>
@@ -7844,10 +7839,10 @@
         <v>COTNCOA1</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E22" s="36">
         <v>2006</v>
@@ -7871,10 +7866,10 @@
       <c r="M22" s="114"/>
       <c r="N22" s="114"/>
       <c r="O22" s="114" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="P22" s="121" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Q22" s="114" t="s">
         <v>52</v>
@@ -7892,10 +7887,10 @@
         <v>COTNGAS1</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E23" s="36">
         <v>2006</v>
@@ -7919,10 +7914,10 @@
       <c r="M23" s="114"/>
       <c r="N23" s="114"/>
       <c r="O23" s="114" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P23" s="121" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="Q23" s="114" t="s">
         <v>52</v>
@@ -7940,10 +7935,10 @@
         <v>COTNOIL1</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E24" s="36">
         <v>2006</v>
@@ -7966,10 +7961,10 @@
       <c r="M24" s="114"/>
       <c r="N24" s="114"/>
       <c r="O24" s="114" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P24" s="121" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q24" s="114" t="s">
         <v>52</v>
@@ -7987,10 +7982,10 @@
         <v>COTNBIO1</v>
       </c>
       <c r="C25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" s="36">
         <v>2006</v>
@@ -8013,10 +8008,10 @@
       <c r="M25" s="114"/>
       <c r="N25" s="114"/>
       <c r="O25" s="114" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P25" s="121" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="Q25" s="114" t="s">
         <v>52</v>
@@ -8034,10 +8029,10 @@
         <v>COTNELC1</v>
       </c>
       <c r="C26" s="98" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D26" s="98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E26" s="99">
         <v>2006</v>
@@ -8061,10 +8056,10 @@
       <c r="M26" s="122"/>
       <c r="N26" s="122"/>
       <c r="O26" s="122" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P26" s="123" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q26" s="122" t="s">
         <v>52</v>
@@ -8082,10 +8077,10 @@
         <v>RSHNCOA1</v>
       </c>
       <c r="C27" s="102" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" s="102" t="s">
         <v>172</v>
-      </c>
-      <c r="D27" s="102" t="s">
-        <v>173</v>
       </c>
       <c r="E27" s="36">
         <v>2006</v>
@@ -8111,10 +8106,10 @@
       <c r="M27" s="116"/>
       <c r="N27" s="116"/>
       <c r="O27" s="115" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="P27" s="121" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q27" s="114" t="s">
         <v>52</v>
@@ -8135,7 +8130,7 @@
         <v>98</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E28" s="36">
         <v>2006</v>
@@ -8162,10 +8157,10 @@
       <c r="M28" s="116"/>
       <c r="N28" s="116"/>
       <c r="O28" s="115" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="P28" s="121" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q28" s="114" t="s">
         <v>52</v>
@@ -8183,10 +8178,10 @@
         <v>RSHNOIL1</v>
       </c>
       <c r="C29" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E29" s="36">
         <v>2006</v>
@@ -8213,10 +8208,10 @@
       <c r="M29" s="116"/>
       <c r="N29" s="116"/>
       <c r="O29" s="115" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P29" s="121" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q29" s="114" t="s">
         <v>52</v>
@@ -8234,10 +8229,10 @@
         <v>RSHNBIO1</v>
       </c>
       <c r="C30" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E30" s="36">
         <v>2006</v>
@@ -8264,10 +8259,10 @@
       <c r="M30" s="116"/>
       <c r="N30" s="116"/>
       <c r="O30" s="115" t="s">
+        <v>214</v>
+      </c>
+      <c r="P30" s="121" t="s">
         <v>215</v>
-      </c>
-      <c r="P30" s="121" t="s">
-        <v>216</v>
       </c>
       <c r="Q30" s="114" t="s">
         <v>52</v>
@@ -8285,10 +8280,10 @@
         <v>RSHNSOL1</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E31" s="36">
         <v>2006</v>
@@ -8315,10 +8310,10 @@
       <c r="M31" s="116"/>
       <c r="N31" s="116"/>
       <c r="O31" s="115" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P31" s="121" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q31" s="114" t="s">
         <v>52</v>
@@ -8336,10 +8331,10 @@
         <v>RSHNELC1</v>
       </c>
       <c r="C32" s="86" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D32" s="86" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E32" s="36">
         <v>2006</v>
@@ -8366,10 +8361,10 @@
       <c r="M32" s="116"/>
       <c r="N32" s="116"/>
       <c r="O32" s="115" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P32" s="121" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="Q32" s="114" t="s">
         <v>52</v>
@@ -8387,10 +8382,10 @@
         <v>RAPNELC1</v>
       </c>
       <c r="C33" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="87" t="s">
         <v>175</v>
-      </c>
-      <c r="D33" s="87" t="s">
-        <v>176</v>
       </c>
       <c r="E33" s="93">
         <v>2006</v>
@@ -8415,10 +8410,10 @@
       <c r="M33" s="116"/>
       <c r="N33" s="116"/>
       <c r="O33" s="115" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P33" s="121" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q33" s="114" t="s">
         <v>52</v>
@@ -8436,7 +8431,7 @@
         <v>ROTNCOA1</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" s="35" t="s">
         <v>95</v>
@@ -8464,10 +8459,10 @@
       <c r="M34" s="116"/>
       <c r="N34" s="116"/>
       <c r="O34" s="115" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="P34" s="121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="Q34" s="114" t="s">
         <v>52</v>
@@ -8513,10 +8508,10 @@
       <c r="M35" s="116"/>
       <c r="N35" s="116"/>
       <c r="O35" s="115" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="P35" s="121" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="Q35" s="114" t="s">
         <v>52</v>
@@ -8534,7 +8529,7 @@
         <v>ROTNOIL1</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D36" s="35" t="s">
         <v>95</v>
@@ -8561,10 +8556,10 @@
       <c r="M36" s="116"/>
       <c r="N36" s="116"/>
       <c r="O36" s="115" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P36" s="121" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Q36" s="114" t="s">
         <v>52</v>
@@ -8582,7 +8577,7 @@
         <v>ROTNBIO1</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>95</v>
@@ -8609,10 +8604,10 @@
       <c r="M37" s="116"/>
       <c r="N37" s="116"/>
       <c r="O37" s="115" t="s">
+        <v>227</v>
+      </c>
+      <c r="P37" s="121" t="s">
         <v>228</v>
-      </c>
-      <c r="P37" s="121" t="s">
-        <v>229</v>
       </c>
       <c r="Q37" s="114" t="s">
         <v>52</v>
@@ -8630,7 +8625,7 @@
         <v>ROTNELC1</v>
       </c>
       <c r="C38" s="98" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D38" s="98" t="s">
         <v>95</v>
@@ -8658,10 +8653,10 @@
       <c r="M38" s="116"/>
       <c r="N38" s="116"/>
       <c r="O38" s="115" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="P38" s="121" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q38" s="114" t="s">
         <v>52</v>
@@ -8811,15 +8806,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="B1:V25"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -8843,7 +8838,7 @@
     <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="49" t="s">
         <v>43</v>
       </c>
@@ -8867,7 +8862,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B2" s="51" t="s">
         <v>99</v>
       </c>
@@ -8902,7 +8897,7 @@
       <c r="U2" s="109"/>
       <c r="V2" s="109"/>
     </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="N3" s="110" t="s">
         <v>8</v>
       </c>
@@ -8931,7 +8926,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:22" s="8" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="8" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
       <c r="D4" s="50"/>
@@ -8966,7 +8961,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:22" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
       <c r="D5" s="50"/>
@@ -8982,7 +8977,7 @@
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -9003,7 +8998,10 @@
       <c r="U8" s="116"/>
       <c r="V8" s="116"/>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>257</v>
+      </c>
       <c r="B9" s="14" t="s">
         <v>1</v>
       </c>
@@ -9020,10 +9018,10 @@
         <v>17</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>107</v>
+        <v>258</v>
       </c>
       <c r="I9" s="18" t="s">
         <v>39</v>
@@ -9035,7 +9033,7 @@
         <v>70</v>
       </c>
       <c r="L9" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M9" s="29"/>
       <c r="N9" s="110" t="s">
@@ -9066,7 +9064,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="60" t="s">
         <v>73</v>
       </c>
@@ -9084,16 +9082,16 @@
         <v>74</v>
       </c>
       <c r="H10" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="I10" s="62" t="s">
         <v>108</v>
-      </c>
-      <c r="I10" s="62" t="s">
-        <v>109</v>
       </c>
       <c r="J10" s="61" t="s">
         <v>40</v>
       </c>
       <c r="K10" s="61" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L10" s="61" t="s">
         <v>38</v>
@@ -9127,7 +9125,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="59" t="s">
         <v>80</v>
       </c>
@@ -9135,25 +9133,25 @@
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
       <c r="F11" s="63" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G11" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="H11" s="64" t="s">
+      <c r="I11" s="64" t="s">
         <v>111</v>
       </c>
-      <c r="I11" s="64" t="s">
+      <c r="J11" s="63" t="s">
         <v>112</v>
-      </c>
-      <c r="J11" s="63" t="s">
-        <v>113</v>
       </c>
       <c r="K11" s="63" t="s">
         <v>84</v>
       </c>
       <c r="L11" s="63" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M11" s="68"/>
       <c r="N11" s="124" t="s">
@@ -9168,16 +9166,19 @@
       <c r="U11" s="125"/>
       <c r="V11" s="125"/>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>113</v>
+      </c>
       <c r="B12" t="str">
         <f>P12</f>
         <v>TCANGAS1</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E12">
         <v>2006</v>
@@ -9209,33 +9210,36 @@
       </c>
       <c r="O12" s="114"/>
       <c r="P12" s="109" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q12" s="109" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R12" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S12" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T12" s="116"/>
       <c r="U12" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V12" s="114"/>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>113</v>
+      </c>
       <c r="B13" t="str">
         <f t="shared" ref="B13:B23" si="0">P13</f>
         <v>TCANDSL1</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E13">
         <v>2006</v>
@@ -9265,33 +9269,36 @@
       <c r="N13" s="114"/>
       <c r="O13" s="114"/>
       <c r="P13" s="109" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q13" s="109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R13" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S13" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T13" s="116"/>
       <c r="U13" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V13" s="114"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>TCANLPG1</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E14">
         <v>2006</v>
@@ -9321,33 +9328,36 @@
       <c r="N14" s="114"/>
       <c r="O14" s="114"/>
       <c r="P14" s="109" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q14" s="109" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R14" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S14" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T14" s="116"/>
       <c r="U14" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V14" s="114"/>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>113</v>
+      </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>TCANGSL1</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15">
         <v>2006</v>
@@ -9377,33 +9387,36 @@
       <c r="N15" s="114"/>
       <c r="O15" s="114"/>
       <c r="P15" s="109" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q15" s="109" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R15" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S15" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T15" s="116"/>
       <c r="U15" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V15" s="114"/>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
       <c r="B16" t="str">
         <f>P16</f>
         <v>TCARNBIO1</v>
       </c>
       <c r="C16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E16">
         <v>2010</v>
@@ -9433,33 +9446,36 @@
       <c r="N16" s="114"/>
       <c r="O16" s="114"/>
       <c r="P16" s="109" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q16" s="109" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="R16" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S16" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T16" s="116"/>
       <c r="U16" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V16" s="114"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>113</v>
+      </c>
       <c r="B17" s="86" t="str">
         <f t="shared" si="0"/>
         <v>TCANELC1</v>
       </c>
       <c r="C17" s="103" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17" s="86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E17" s="86">
         <v>2010</v>
@@ -9490,33 +9506,36 @@
       <c r="N17" s="126"/>
       <c r="O17" s="126"/>
       <c r="P17" s="127" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Q17" s="127" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R17" s="128" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S17" s="128" t="s">
         <v>102</v>
       </c>
       <c r="T17" s="128"/>
       <c r="U17" s="128" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V17" s="126"/>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>113</v>
+      </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>TPUNGAS1</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E18">
         <v>2006</v>
@@ -9545,33 +9564,36 @@
       <c r="N18" s="114"/>
       <c r="O18" s="114"/>
       <c r="P18" s="109" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Q18" s="109" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R18" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S18" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T18" s="116"/>
       <c r="U18" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V18" s="114"/>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>TPUNDSL1</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E19">
         <v>2006</v>
@@ -9600,33 +9622,36 @@
       <c r="N19" s="116"/>
       <c r="O19" s="116"/>
       <c r="P19" s="109" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="Q19" s="109" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R19" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S19" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T19" s="116"/>
       <c r="U19" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V19" s="116"/>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>113</v>
+      </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>TPUNLPG1</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20">
         <v>2006</v>
@@ -9655,33 +9680,36 @@
       <c r="N20" s="116"/>
       <c r="O20" s="116"/>
       <c r="P20" s="109" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="Q20" s="109" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="R20" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S20" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T20" s="116"/>
       <c r="U20" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V20" s="116"/>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>113</v>
+      </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>TPUNGSL1</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E21">
         <v>2006</v>
@@ -9710,33 +9738,36 @@
       <c r="N21" s="116"/>
       <c r="O21" s="116"/>
       <c r="P21" s="109" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="Q21" s="109" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R21" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S21" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T21" s="116"/>
       <c r="U21" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V21" s="116"/>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
       <c r="B22" t="str">
         <f>P22</f>
         <v>TPUBNBIO1</v>
       </c>
       <c r="C22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E22">
         <v>2006</v>
@@ -9765,33 +9796,36 @@
       <c r="N22" s="116"/>
       <c r="O22" s="116"/>
       <c r="P22" s="109" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q22" s="109" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="R22" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S22" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T22" s="116"/>
       <c r="U22" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V22" s="116"/>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>TPUNELC1</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E23">
         <v>2010</v>
@@ -9801,9 +9835,6 @@
       </c>
       <c r="G23">
         <v>15</v>
-      </c>
-      <c r="H23">
-        <v>200</v>
       </c>
       <c r="I23" s="71">
         <v>37.5</v>
@@ -9820,24 +9851,36 @@
       <c r="N23" s="116"/>
       <c r="O23" s="116"/>
       <c r="P23" s="109" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="Q23" s="109" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R23" s="116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="S23" s="116" t="s">
         <v>102</v>
       </c>
       <c r="T23" s="116"/>
       <c r="U23" s="116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V23" s="116"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="str">
+        <f>B23</f>
+        <v>TPUNELC1</v>
+      </c>
+      <c r="H24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="F25" s="67"/>
     </row>
   </sheetData>
@@ -9872,13 +9915,13 @@
   <sheetData>
     <row r="2" spans="2:29" x14ac:dyDescent="0.2">
       <c r="B2" s="107" t="s">
+        <v>203</v>
+      </c>
+      <c r="P2" s="107" t="s">
         <v>204</v>
       </c>
-      <c r="P2" s="107" t="s">
+      <c r="AC2" s="107" t="s">
         <v>205</v>
-      </c>
-      <c r="AC2" s="107" t="s">
-        <v>206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>